<commit_message>
bb fuel upstream can now multipurpose it be used for both biofuels and fossil fuels, if either is connected as a fuel type in a factory connections Using lookup names will propogate from the origin unit process
</commit_message>
<xml_diff>
--- a/data/shared/energy_calc.xlsx
+++ b/data/shared/energy_calc.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\setanzer\GitHub\BlackBlox\data\shared\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/shared/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14CBEC8C-43B9-6243-8888-933724A315EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="555" yWindow="765" windowWidth="24480" windowHeight="17235" tabRatio="799" activeTab="4"/>
+    <workbookView xWindow="740" yWindow="460" windowWidth="24480" windowHeight="17240" tabRatio="799" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Heat Recovery" sheetId="3" r:id="rId1"/>
     <sheet name="bb electricity" sheetId="2" r:id="rId2"/>
     <sheet name="bb heat" sheetId="4" r:id="rId3"/>
-    <sheet name="bb fuel upstream" sheetId="6" r:id="rId4"/>
-    <sheet name="bb biofuel upstream" sheetId="7" r:id="rId5"/>
+    <sheet name="old-bb fuel upstream" sheetId="7" r:id="rId4"/>
+    <sheet name="bb fuel upstream" sheetId="10" r:id="rId5"/>
+    <sheet name="bb biofuel upstream" sheetId="9" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="51">
   <si>
     <t>Combustion</t>
   </si>
@@ -102,9 +104,6 @@
     <t>inflows</t>
   </si>
   <si>
-    <t>carbon and oxygen</t>
-  </si>
-  <si>
     <t>outflows</t>
   </si>
   <si>
@@ -129,47 +128,68 @@
     <t>subtraction</t>
   </si>
   <si>
+    <t>lookup ratio-fuels</t>
+  </si>
+  <si>
+    <t>CO2__emitted</t>
+  </si>
+  <si>
+    <t>CO2__removed from atmosphere</t>
+  </si>
+  <si>
+    <t>CONSUMED carbon and oxygen</t>
+  </si>
+  <si>
+    <t>CO2 removal</t>
+  </si>
+  <si>
+    <t>fuel source ratio</t>
+  </si>
+  <si>
+    <t>CONSUMED embodied CO2 removal</t>
+  </si>
+  <si>
+    <t>fuel production losses</t>
+  </si>
+  <si>
+    <t>biomass</t>
+  </si>
+  <si>
+    <t>biofuel production losses</t>
+  </si>
+  <si>
     <t>biofuel</t>
   </si>
   <si>
-    <t>biomass CO2 absorption</t>
+    <t>temp</t>
+  </si>
+  <si>
+    <t>raw fossil fuel</t>
+  </si>
+  <si>
+    <t>is fossil</t>
+  </si>
+  <si>
+    <t>biomass-to-fuel ratio</t>
+  </si>
+  <si>
+    <t>is biofuel</t>
+  </si>
+  <si>
+    <t>is_biofuel</t>
   </si>
   <si>
     <t>biofuel__biomass</t>
   </si>
   <si>
-    <t>biomass losses</t>
-  </si>
-  <si>
-    <t>fresh biomass</t>
-  </si>
-  <si>
-    <t>energy in biofuel</t>
-  </si>
-  <si>
-    <t>lookup ratio-fuels</t>
-  </si>
-  <si>
-    <t>temp</t>
-  </si>
-  <si>
-    <t>fresh biomass ratio</t>
-  </si>
-  <si>
-    <t>CO2__emitted</t>
-  </si>
-  <si>
-    <t>CO2__removed from atmosphere</t>
-  </si>
-  <si>
-    <t>CONSUMED CO2 removals net emissions</t>
+    <t>biofuel__production losses</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -188,6 +208,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -214,7 +241,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -222,10 +249,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -536,25 +565,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.875" style="1"/>
+    <col min="3" max="3" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -583,7 +612,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
@@ -603,7 +632,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -629,25 +658,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.875" style="1"/>
+    <col min="3" max="3" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -676,7 +705,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -702,16 +731,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -740,7 +769,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -766,25 +795,27 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>10</v>
@@ -814,79 +845,147 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="G2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" t="s">
         <v>19</v>
       </c>
-      <c r="E3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
         <v>23</v>
       </c>
       <c r="F5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
         <v>22</v>
       </c>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -894,26 +993,27 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A70F89E-5DC9-0C49-8530-3AA9CB13A34B}">
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="10.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>10</v>
@@ -943,148 +1043,417 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
         <v>33</v>
       </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" t="s">
-        <v>36</v>
-      </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
         <v>32</v>
       </c>
-      <c r="H4" t="s">
+      <c r="G4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
         <v>33</v>
       </c>
-      <c r="I4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>37</v>
-      </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
         <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="F5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" t="s">
         <v>43</v>
       </c>
-      <c r="E6" t="s">
-        <v>23</v>
-      </c>
       <c r="F6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
         <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="F7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" t="s">
         <v>43</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" t="s">
         <v>23</v>
-      </c>
-      <c r="D8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" t="s">
-        <v>25</v>
       </c>
       <c r="F8" t="s">
         <v>32</v>
       </c>
-      <c r="H8" t="s">
+      <c r="G8" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" t="s">
         <v>42</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A64EE393-54BE-CE45-9B4D-22F06B6E4714}">
+  <dimension ref="A1:J12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" t="s">
         <v>25</v>
       </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>